<commit_message>
Age, EducationLevel and GameLevel Anova
</commit_message>
<xml_diff>
--- a/CIF/CIF_Data.xlsx
+++ b/CIF/CIF_Data.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="100">
   <si>
     <t xml:space="preserve">BODY FUNCTIONS </t>
   </si>
@@ -997,7 +997,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1009,10 +1057,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1024,37 +1069,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1062,21 +1077,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1429,8 +1429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1449,24 +1449,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="81"/>
+      <c r="A1" s="59"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="61" t="s">
+      <c r="C1" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="62"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="78"/>
     </row>
     <row r="2" spans="1:11" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="81"/>
+      <c r="A2" s="59"/>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1531,54 +1531,54 @@
       <c r="K4" s="14"/>
     </row>
     <row r="5" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="63" t="s">
+      <c r="A5" s="66" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="15"/>
-      <c r="C5" s="82"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="83" t="s">
+      <c r="C5" s="79"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="60" t="s">
         <v>99</v>
       </c>
-      <c r="I5" s="65"/>
-      <c r="J5" s="65"/>
-      <c r="K5" s="66"/>
+      <c r="I5" s="80"/>
+      <c r="J5" s="80"/>
+      <c r="K5" s="81"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="64"/>
+      <c r="A6" s="67"/>
       <c r="B6" s="15"/>
-      <c r="C6" s="82"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="65"/>
-      <c r="H6" s="83" t="s">
+      <c r="C6" s="79"/>
+      <c r="D6" s="80"/>
+      <c r="E6" s="80"/>
+      <c r="F6" s="80"/>
+      <c r="G6" s="80"/>
+      <c r="H6" s="60" t="s">
         <v>99</v>
       </c>
-      <c r="I6" s="65"/>
-      <c r="J6" s="65"/>
-      <c r="K6" s="66"/>
+      <c r="I6" s="80"/>
+      <c r="J6" s="80"/>
+      <c r="K6" s="81"/>
     </row>
     <row r="7" spans="1:11" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="64"/>
+      <c r="A7" s="67"/>
       <c r="B7" s="16"/>
-      <c r="C7" s="82"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="65"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="65"/>
-      <c r="H7" s="83" t="s">
+      <c r="C7" s="79"/>
+      <c r="D7" s="80"/>
+      <c r="E7" s="80"/>
+      <c r="F7" s="80"/>
+      <c r="G7" s="80"/>
+      <c r="H7" s="60" t="s">
         <v>99</v>
       </c>
-      <c r="I7" s="65"/>
-      <c r="J7" s="65"/>
-      <c r="K7" s="66"/>
+      <c r="I7" s="80"/>
+      <c r="J7" s="80"/>
+      <c r="K7" s="81"/>
     </row>
     <row r="8" spans="1:11" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="74" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="15"/>
@@ -1597,7 +1597,7 @@
       <c r="K8" s="58"/>
     </row>
     <row r="9" spans="1:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="60"/>
+      <c r="A9" s="76"/>
       <c r="B9" s="15"/>
       <c r="C9" s="17" t="s">
         <v>18</v>
@@ -1607,14 +1607,12 @@
       <c r="F9" s="57"/>
       <c r="G9" s="57"/>
       <c r="H9" s="57"/>
-      <c r="I9" s="18" t="s">
-        <v>18</v>
-      </c>
+      <c r="I9" s="18"/>
       <c r="J9" s="57"/>
       <c r="K9" s="58"/>
     </row>
     <row r="10" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="67" t="s">
+      <c r="A10" s="82" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="15" t="s">
@@ -1631,7 +1629,7 @@
       <c r="K10" s="58"/>
     </row>
     <row r="11" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="68"/>
+      <c r="A11" s="64"/>
       <c r="B11" s="15" t="s">
         <v>22</v>
       </c>
@@ -1646,7 +1644,7 @@
       <c r="K11" s="58"/>
     </row>
     <row r="12" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="69"/>
+      <c r="A12" s="83"/>
       <c r="B12" s="15" t="s">
         <v>22</v>
       </c>
@@ -1661,7 +1659,7 @@
       <c r="K12" s="58"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="70" t="s">
+      <c r="A13" s="69" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="15"/>
@@ -1693,7 +1691,7 @@
       <c r="K14" s="58"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="59" t="s">
+      <c r="A15" s="74" t="s">
         <v>25</v>
       </c>
       <c r="B15" s="15" t="s">
@@ -1710,7 +1708,7 @@
       <c r="K15" s="58"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="60"/>
+      <c r="A16" s="76"/>
       <c r="B16" s="16"/>
       <c r="C16" s="19" t="s">
         <v>26</v>
@@ -1748,7 +1746,7 @@
       <c r="K17" s="58"/>
     </row>
     <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="59" t="s">
+      <c r="A18" s="74" t="s">
         <v>32</v>
       </c>
       <c r="B18" s="15"/>
@@ -1767,7 +1765,7 @@
       <c r="K18" s="58"/>
     </row>
     <row r="19" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="60"/>
+      <c r="A19" s="76"/>
       <c r="B19" s="15"/>
       <c r="C19" s="19"/>
       <c r="D19" s="57"/>
@@ -1784,7 +1782,7 @@
       <c r="K19" s="58"/>
     </row>
     <row r="20" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="63" t="s">
+      <c r="A20" s="66" t="s">
         <v>34</v>
       </c>
       <c r="B20" s="15"/>
@@ -1801,7 +1799,7 @@
       <c r="K20" s="58"/>
     </row>
     <row r="21" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="64"/>
+      <c r="A21" s="67"/>
       <c r="B21" s="15"/>
       <c r="C21" s="19"/>
       <c r="D21" s="57"/>
@@ -1871,7 +1869,7 @@
       <c r="K24" s="58"/>
     </row>
     <row r="25" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="63" t="s">
+      <c r="A25" s="66" t="s">
         <v>40</v>
       </c>
       <c r="B25" s="15" t="s">
@@ -1888,7 +1886,7 @@
       <c r="K25" s="58"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="64"/>
+      <c r="A26" s="67"/>
       <c r="B26" s="15"/>
       <c r="C26" s="19"/>
       <c r="D26" s="57"/>
@@ -1905,7 +1903,7 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="74"/>
+      <c r="A27" s="68"/>
       <c r="B27" s="15" t="s">
         <v>44</v>
       </c>
@@ -1920,7 +1918,7 @@
       <c r="K27" s="58"/>
     </row>
     <row r="28" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="70" t="s">
+      <c r="A28" s="69" t="s">
         <v>45</v>
       </c>
       <c r="B28" s="15" t="s">
@@ -1937,7 +1935,7 @@
       <c r="K28" s="58"/>
     </row>
     <row r="29" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="75"/>
+      <c r="A29" s="70"/>
       <c r="B29" s="15" t="s">
         <v>47</v>
       </c>
@@ -2022,7 +2020,7 @@
       <c r="G33" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="H33" s="81"/>
+      <c r="H33" s="59"/>
       <c r="I33" s="57"/>
       <c r="J33" s="57"/>
       <c r="K33" s="58" t="s">
@@ -2070,7 +2068,7 @@
       </c>
     </row>
     <row r="36" spans="1:11" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="76" t="s">
+      <c r="A36" s="72" t="s">
         <v>60</v>
       </c>
       <c r="B36" s="30"/>
@@ -2093,7 +2091,7 @@
       </c>
     </row>
     <row r="37" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="77"/>
+      <c r="A37" s="73"/>
       <c r="B37" s="30"/>
       <c r="C37" s="19" t="s">
         <v>61</v>
@@ -2114,7 +2112,7 @@
       </c>
     </row>
     <row r="38" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="63" t="s">
+      <c r="A38" s="66" t="s">
         <v>63</v>
       </c>
       <c r="B38" s="15"/>
@@ -2139,7 +2137,7 @@
       </c>
     </row>
     <row r="39" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="74"/>
+      <c r="A39" s="68"/>
       <c r="B39" s="15" t="s">
         <v>44</v>
       </c>
@@ -2154,7 +2152,7 @@
       <c r="K39" s="29"/>
     </row>
     <row r="40" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="59" t="s">
+      <c r="A40" s="74" t="s">
         <v>68</v>
       </c>
       <c r="B40" s="15"/>
@@ -2175,7 +2173,7 @@
       <c r="K40" s="58"/>
     </row>
     <row r="41" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="78"/>
+      <c r="A41" s="75"/>
       <c r="B41" s="15"/>
       <c r="C41" s="26"/>
       <c r="D41" s="57"/>
@@ -2194,11 +2192,11 @@
       <c r="K41" s="58"/>
     </row>
     <row r="42" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="72" t="s">
+      <c r="A42" s="63" t="s">
         <v>71</v>
       </c>
       <c r="B42" s="15"/>
-      <c r="C42" s="84"/>
+      <c r="C42" s="61"/>
       <c r="D42" s="57"/>
       <c r="E42" s="57" t="s">
         <v>72</v>
@@ -2217,9 +2215,9 @@
       </c>
     </row>
     <row r="43" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="68"/>
+      <c r="A43" s="64"/>
       <c r="B43" s="15"/>
-      <c r="C43" s="84"/>
+      <c r="C43" s="61"/>
       <c r="D43" s="57"/>
       <c r="E43" s="57" t="s">
         <v>72</v>
@@ -2238,9 +2236,9 @@
       </c>
     </row>
     <row r="44" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="73"/>
+      <c r="A44" s="65"/>
       <c r="B44" s="31"/>
-      <c r="C44" s="85"/>
+      <c r="C44" s="62"/>
       <c r="D44" s="32"/>
       <c r="E44" s="32" t="s">
         <v>75</v>
@@ -2264,13 +2262,6 @@
     <row r="47" spans="1:11" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A41"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="C1:K1"/>
     <mergeCell ref="A5:A7"/>
@@ -2286,6 +2277,13 @@
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2579,15 +2577,15 @@
       <c r="B4" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="E4" s="80"/>
-      <c r="F4" s="79"/>
-      <c r="G4" s="79"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="84"/>
+      <c r="G4" s="84"/>
       <c r="H4" s="44"/>
       <c r="I4" s="44"/>
       <c r="J4" s="44"/>
-      <c r="K4" s="79"/>
-      <c r="L4" s="79"/>
-      <c r="M4" s="79"/>
+      <c r="K4" s="84"/>
+      <c r="L4" s="84"/>
+      <c r="M4" s="84"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="39" t="s">
@@ -2596,15 +2594,15 @@
       <c r="B5" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="E5" s="80"/>
-      <c r="F5" s="79"/>
-      <c r="G5" s="79"/>
-      <c r="H5" s="79"/>
-      <c r="I5" s="79"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="84"/>
+      <c r="H5" s="84"/>
+      <c r="I5" s="84"/>
       <c r="J5" s="46"/>
-      <c r="K5" s="79"/>
-      <c r="L5" s="79"/>
-      <c r="M5" s="79"/>
+      <c r="K5" s="84"/>
+      <c r="L5" s="84"/>
+      <c r="M5" s="84"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="39" t="s">
@@ -2613,15 +2611,15 @@
       <c r="B6" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="80"/>
-      <c r="F6" s="79"/>
-      <c r="G6" s="79"/>
-      <c r="H6" s="79"/>
-      <c r="I6" s="79"/>
+      <c r="E6" s="85"/>
+      <c r="F6" s="84"/>
+      <c r="G6" s="84"/>
+      <c r="H6" s="84"/>
+      <c r="I6" s="84"/>
       <c r="J6" s="46"/>
-      <c r="K6" s="79"/>
-      <c r="L6" s="79"/>
-      <c r="M6" s="79"/>
+      <c r="K6" s="84"/>
+      <c r="L6" s="84"/>
+      <c r="M6" s="84"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="39" t="s">
@@ -2632,8 +2630,8 @@
       </c>
       <c r="F7" s="44"/>
       <c r="G7" s="44"/>
-      <c r="H7" s="79"/>
-      <c r="I7" s="79"/>
+      <c r="H7" s="84"/>
+      <c r="I7" s="84"/>
       <c r="J7" s="46"/>
       <c r="K7" s="44"/>
       <c r="L7" s="44"/>

</xml_diff>